<commit_message>
Export to GHG Tool working
</commit_message>
<xml_diff>
--- a/collect-earth/collect-earth-app/src/main/java/org/openforis/collect/earth/ipcc/serialize/IPCC2006_nomenclatures.xlsx
+++ b/collect-earth/collect-earth-app/src/main/java/org/openforis/collect/earth/ipcc/serialize/IPCC2006_nomenclatures.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\IPCC2006\doc\CollectEarth\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfonso Sanchez-Paus\workspace\maven.1480939002496\collect-earth\collect-earth-app\src\main\java\org\openforis\collect\earth\ipcc\serialize\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4A1C5D-4977-431B-9E2B-B6F620D13D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10785"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries" sheetId="1" r:id="rId1"/>
@@ -43,32 +44,32 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" sourceFile="D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb" keepAlive="1" name="ipcc2006_unprotected" type="5" refreshedVersion="5" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" sourceFile="D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb" keepAlive="1" name="ipcc2006_unprotected" type="5" refreshedVersion="5" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.ACE.OLEDB.12.0;User ID=Admin;Data Source=D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb;Mode=Share Deny Write;Extended Properties=&quot;&quot;;Jet OLEDB:System database=&quot;&quot;;Jet OLEDB:Registry Path=&quot;&quot;;Jet OLEDB:Engine Type=6;Jet OLEDB:Database Locking Mode=0;Jet OLEDB:Global Partial Bulk Ops=2;Jet OLEDB:Global Bulk Transactions=1;Jet OLEDB:New Database Password=&quot;&quot;;Jet OLEDB:Create System Database=False;Jet OLEDB:Encrypt Database=False;Jet OLEDB:Don't Copy Locale on Compact=False;Jet OLEDB:Compact Without Replica Repair=False;Jet OLEDB:SFP=False;Jet OLEDB:Support Complex Data=False;Jet OLEDB:Bypass UserInfo Validation=False;Jet OLEDB:Limited DB Caching=False;Jet OLEDB:Bypass ChoiceField Validation=False" command="country" commandType="3"/>
   </connection>
-  <connection id="2" name="Query from IPCC2006" type="1" refreshedVersion="5" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="Query from IPCC2006" type="1" refreshedVersion="5" background="1" saveData="1">
     <dbPr connection="DSN=IPCC2006;DBQ=D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb;DriverId=25;FIL=MS Access;MaxBufferSize=2048;PageTimeout=5;" command="SELECT cl_climate_region.ID, cl_climate_region.domain_id, cl_climate_region.region, cl_climate_region.country_code, cl_climate_region.GUID_x000d__x000a_FROM `D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb`.cl_climate_region cl_climate_region_x000d__x000a_ORDER BY cl_climate_region.ID"/>
   </connection>
-  <connection id="3" name="Query from IPCC20061" type="1" refreshedVersion="5" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="Query from IPCC20061" type="1" refreshedVersion="5" background="1" saveData="1">
     <dbPr connection="DSN=IPCC2006;DBQ=D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb;DriverId=25;FIL=MS Access;MaxBufferSize=2048;PageTimeout=5;" command="SELECT cl_climate_domain.ID, cl_climate_domain.domain_x000d__x000a_FROM `D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb`.cl_climate_domain cl_climate_domain_x000d__x000a_ORDER BY cl_climate_domain.ID"/>
   </connection>
-  <connection id="4" name="Query from IPCC20062" type="1" refreshedVersion="5" background="1" saveData="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="Query from IPCC20062" type="1" refreshedVersion="5" background="1" saveData="1">
     <dbPr connection="DSN=IPCC2006;DBQ=D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb;DriverId=25;FIL=MS Access;MaxBufferSize=2048;PageTimeout=5;" command="SELECT cl_soil_type.ID, cl_soil_type.full_name, cl_soil_type.composition_id, cl_soil_type.GUID_x000d__x000a_FROM `D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb`.cl_soil_type cl_soil_type_x000d__x000a_ORDER BY cl_soil_type.ID"/>
   </connection>
-  <connection id="5" name="Query from IPCC20063" type="1" refreshedVersion="5" background="1" saveData="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="Query from IPCC20063" type="1" refreshedVersion="5" background="1" saveData="1">
     <dbPr connection="DSN=IPCC2006;DBQ=D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb;DriverId=25;FIL=MS Access;MaxBufferSize=2048;PageTimeout=5;" command="SELECT cl_soil_composition.ID, cl_soil_composition.composition_x000d__x000a_FROM `D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb`.cl_soil_composition cl_soil_composition_x000d__x000a_ORDER BY cl_soil_composition.ID"/>
   </connection>
-  <connection id="6" name="Query from IPCC20064" type="1" refreshedVersion="5" background="1" saveData="1">
+  <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" name="Query from IPCC20064" type="1" refreshedVersion="5" background="1" saveData="1">
     <dbPr connection="DSN=IPCC2006;DBQ=D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb;DriverId=25;FIL=MS Access;MaxBufferSize=2048;PageTimeout=5;" command="SELECT cl_soil_status.ID, cl_soil_status.name_x000d__x000a_FROM `D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb`.cl_soil_status cl_soil_status_x000d__x000a_ORDER BY cl_soil_status.ID"/>
   </connection>
-  <connection id="7" name="Query from IPCC20065" type="1" refreshedVersion="5" background="1" saveData="1">
+  <connection id="7" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" name="Query from IPCC20065" type="1" refreshedVersion="5" background="1" saveData="1">
     <dbPr connection="DSN=IPCC2006;DBQ=D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb;DriverId=25;FIL=MS Access;MaxBufferSize=2048;PageTimeout=5;" command="SELECT cl_nutrient_type.ID, cl_nutrient_type.nutrient_type, cl_nutrient_type.description_x000d__x000a_FROM `D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb`.cl_nutrient_type cl_nutrient_type_x000d__x000a_ORDER BY cl_nutrient_type.ID"/>
   </connection>
-  <connection id="8" name="Query from IPCC20066" type="1" refreshedVersion="5" background="1" saveData="1">
+  <connection id="8" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" name="Query from IPCC20066" type="1" refreshedVersion="5" background="1" saveData="1">
     <dbPr connection="DSN=IPCC2006;DBQ=D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb;DriverId=25;FIL=MS Access;MaxBufferSize=2048;PageTimeout=5;" command="SELECT cl_land_type.ID, cl_land_type.ipcc_code, cl_land_type.type_name, cl_land_type.abbr_x000d__x000a_FROM `D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb`.cl_land_type cl_land_type_x000d__x000a_ORDER BY cl_land_type.ID"/>
   </connection>
-  <connection id="9" name="Query from IPCC20067" type="1" refreshedVersion="5" background="1" saveData="1">
+  <connection id="9" xr16:uid="{00000000-0015-0000-FFFF-FFFF08000000}" name="Query from IPCC20067" type="1" refreshedVersion="5" background="1" saveData="1">
     <dbPr connection="DSN=IPCC2006;DBQ=D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb;DriverId=25;FIL=MS Access;MaxBufferSize=2048;PageTimeout=5;" command="SELECT cl_land_type_subcategory.ID, cl_land_type_subcategory.lt_id, cl_land_type_subcategory.name, cl_land_type_subcategory.abbr_x000d__x000a_FROM `D:\Projects\IPCC2006\db\ipcc2006_unprotected.accdb`.cl_land_type_subcategory cl_land_type_subcategory_x000d__x000a_ORDER BY cl_land_type_subcategory.ID"/>
   </connection>
 </connections>
@@ -1913,7 +1914,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1964,7 +1965,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ipcc2006_unprotected.accdb" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ipcc2006_unprotected.accdb" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4">
     <queryTableFields count="2">
       <queryTableField id="1" name="country_code" tableColumnId="1"/>
@@ -1978,7 +1979,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Query from IPCC2006_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Query from IPCC2006_1" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="6">
     <queryTableFields count="5">
       <queryTableField id="1" name="ID" tableColumnId="1"/>
@@ -1992,7 +1993,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Query from IPCC2006" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Query from IPCC2006" connectionId="3" xr16:uid="{00000000-0016-0000-0200-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="3">
     <queryTableFields count="2">
       <queryTableField id="1" name="ID" tableColumnId="1"/>
@@ -2003,7 +2004,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Query from IPCC2006" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Query from IPCC2006" connectionId="4" xr16:uid="{00000000-0016-0000-0300-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="5">
     <queryTableFields count="4">
       <queryTableField id="1" name="ID" tableColumnId="1"/>
@@ -2016,7 +2017,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Query from IPCC2006" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Query from IPCC2006" connectionId="5" xr16:uid="{00000000-0016-0000-0400-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="3">
     <queryTableFields count="2">
       <queryTableField id="1" name="ID" tableColumnId="1"/>
@@ -2027,7 +2028,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Query from IPCC2006" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Query from IPCC2006" connectionId="6" xr16:uid="{00000000-0016-0000-0500-000005000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="3">
     <queryTableFields count="2">
       <queryTableField id="1" name="ID" tableColumnId="1"/>
@@ -2038,7 +2039,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Query from IPCC2006" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Query from IPCC2006" connectionId="7" xr16:uid="{00000000-0016-0000-0600-000006000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4">
     <queryTableFields count="3">
       <queryTableField id="1" name="ID" tableColumnId="1"/>
@@ -2050,7 +2051,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Query from IPCC2006" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Query from IPCC2006" connectionId="8" xr16:uid="{00000000-0016-0000-0700-000007000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="5">
     <queryTableFields count="4">
       <queryTableField id="1" name="ID" tableColumnId="1"/>
@@ -2063,7 +2064,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Query from IPCC2006" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Query from IPCC2006" connectionId="9" xr16:uid="{00000000-0016-0000-0800-000008000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="5">
     <queryTableFields count="4">
       <queryTableField id="1" name="ID" tableColumnId="1"/>
@@ -2076,109 +2077,109 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_ipcc2006_unprotected.accdb" displayName="Table_ipcc2006_unprotected.accdb" ref="A1:B250" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B250"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_ipcc2006_unprotected.accdb" displayName="Table_ipcc2006_unprotected.accdb" ref="A1:B250" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:B250" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="country_code" queryTableFieldId="1"/>
-    <tableColumn id="3" uniqueName="3" name="country_name" queryTableFieldId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="country_code" queryTableFieldId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="country_name" queryTableFieldId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table_Query_from_IPCC2006_1" displayName="Table_Query_from_IPCC2006_1" ref="A1:E18" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_Query_from_IPCC2006_1" displayName="Table_Query_from_IPCC2006_1" ref="A1:E18" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:E18" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" uniqueName="1" name="ID" queryTableFieldId="1"/>
-    <tableColumn id="2" uniqueName="2" name="domain_id" queryTableFieldId="2"/>
-    <tableColumn id="3" uniqueName="3" name="region" queryTableFieldId="3"/>
-    <tableColumn id="4" uniqueName="4" name="country_code" queryTableFieldId="4"/>
-    <tableColumn id="5" uniqueName="5" name="GUID" queryTableFieldId="5"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" uniqueName="1" name="ID" queryTableFieldId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" uniqueName="2" name="domain_id" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" uniqueName="3" name="region" queryTableFieldId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" uniqueName="4" name="country_code" queryTableFieldId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" uniqueName="5" name="GUID" queryTableFieldId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table_Query_from_IPCC2006" displayName="Table_Query_from_IPCC2006" ref="A1:B6" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_Query_from_IPCC2006" displayName="Table_Query_from_IPCC2006" ref="A1:B6" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:B6" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="ID" queryTableFieldId="1"/>
-    <tableColumn id="2" uniqueName="2" name="domain" queryTableFieldId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" uniqueName="1" name="ID" queryTableFieldId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" uniqueName="2" name="domain" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table_Query_from_IPCC20067" displayName="Table_Query_from_IPCC20067" ref="A1:D12" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_Query_from_IPCC20067" displayName="Table_Query_from_IPCC20067" ref="A1:D12" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D12" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" uniqueName="1" name="ID" queryTableFieldId="1"/>
-    <tableColumn id="2" uniqueName="2" name="full_name" queryTableFieldId="2"/>
-    <tableColumn id="3" uniqueName="3" name="composition_id" queryTableFieldId="3"/>
-    <tableColumn id="4" uniqueName="4" name="GUID" queryTableFieldId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" uniqueName="1" name="ID" queryTableFieldId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" uniqueName="2" name="full_name" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" uniqueName="3" name="composition_id" queryTableFieldId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" uniqueName="4" name="GUID" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Query_from_IPCC20068" displayName="Table_Query_from_IPCC20068" ref="A1:B4" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_Query_from_IPCC20068" displayName="Table_Query_from_IPCC20068" ref="A1:B4" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:B4" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="ID" queryTableFieldId="1"/>
-    <tableColumn id="2" uniqueName="2" name="composition" queryTableFieldId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" uniqueName="1" name="ID" queryTableFieldId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" uniqueName="2" name="composition" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Query_from_IPCC20069" displayName="Table_Query_from_IPCC20069" ref="A1:B6" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_Query_from_IPCC20069" displayName="Table_Query_from_IPCC20069" ref="A1:B6" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:B6" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="ID" queryTableFieldId="1"/>
-    <tableColumn id="2" uniqueName="2" name="name" queryTableFieldId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" uniqueName="1" name="ID" queryTableFieldId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" uniqueName="2" name="name" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table_Query_from_IPCC200610" displayName="Table_Query_from_IPCC200610" ref="A1:C4" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table_Query_from_IPCC200610" displayName="Table_Query_from_IPCC200610" ref="A1:C4" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C4" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" uniqueName="1" name="ID" queryTableFieldId="1"/>
-    <tableColumn id="2" uniqueName="2" name="nutrient_type" queryTableFieldId="2"/>
-    <tableColumn id="3" uniqueName="3" name="description" queryTableFieldId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" uniqueName="1" name="ID" queryTableFieldId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" uniqueName="2" name="nutrient_type" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" uniqueName="3" name="description" queryTableFieldId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table_Query_from_IPCC200611" displayName="Table_Query_from_IPCC200611" ref="A1:D7" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table_Query_from_IPCC200611" displayName="Table_Query_from_IPCC200611" ref="A1:D7" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D7" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" uniqueName="1" name="ID" queryTableFieldId="1"/>
-    <tableColumn id="2" uniqueName="2" name="ipcc_code" queryTableFieldId="2"/>
-    <tableColumn id="3" uniqueName="3" name="type_name" queryTableFieldId="3"/>
-    <tableColumn id="4" uniqueName="4" name="abbr" queryTableFieldId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" uniqueName="1" name="ID" queryTableFieldId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" uniqueName="2" name="ipcc_code" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" uniqueName="3" name="type_name" queryTableFieldId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" uniqueName="4" name="abbr" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table_Query_from_IPCC200612" displayName="Table_Query_from_IPCC200612" ref="A1:D13" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table_Query_from_IPCC200612" displayName="Table_Query_from_IPCC200612" ref="A1:D13" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D13" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" uniqueName="1" name="ID" queryTableFieldId="1"/>
-    <tableColumn id="2" uniqueName="2" name="lt_id" queryTableFieldId="2"/>
-    <tableColumn id="3" uniqueName="3" name="name" queryTableFieldId="3"/>
-    <tableColumn id="4" uniqueName="4" name="abbr" queryTableFieldId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" uniqueName="1" name="ID" queryTableFieldId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" uniqueName="2" name="lt_id" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" uniqueName="3" name="name" queryTableFieldId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" uniqueName="4" name="abbr" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2446,10 +2447,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B250"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4466,7 +4467,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4724,7 +4725,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4792,7 +4793,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4965,7 +4966,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5017,10 +5018,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5085,7 +5086,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5148,7 +5149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5268,7 +5269,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
added more access tables
</commit_message>
<xml_diff>
--- a/collect-earth/collect-earth-app/src/main/java/org/openforis/collect/earth/ipcc/serialize/IPCC2006_nomenclatures.xlsx
+++ b/collect-earth/collect-earth-app/src/main/java/org/openforis/collect/earth/ipcc/serialize/IPCC2006_nomenclatures.xlsx
@@ -8,40 +8,52 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfonso Sanchez-Paus\workspace\maven.1480939002496\collect-earth\collect-earth-app\src\main\java\org\openforis\collect\earth\ipcc\serialize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1890FA32-6D5E-4060-97D1-5A568766D846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4650624-4E30-42AA-9DED-D35778FCC785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries" sheetId="1" r:id="rId1"/>
-    <sheet name="Age Classes" sheetId="14" r:id="rId2"/>
-    <sheet name="Perennial Cropland Tyoe" sheetId="15" r:id="rId3"/>
-    <sheet name="Continent Type" sheetId="13" r:id="rId4"/>
-    <sheet name="Eco Zones" sheetId="12" r:id="rId5"/>
-    <sheet name="ClimateRegions" sheetId="3" r:id="rId6"/>
-    <sheet name="ClimateDomains" sheetId="4" r:id="rId7"/>
-    <sheet name="SoilTypes" sheetId="5" r:id="rId8"/>
-    <sheet name="SoilComposition" sheetId="6" r:id="rId9"/>
-    <sheet name="SoilStatus" sheetId="8" r:id="rId10"/>
-    <sheet name="NutrientType" sheetId="9" r:id="rId11"/>
-    <sheet name="LandCategories" sheetId="11" r:id="rId12"/>
-    <sheet name="LandSubcategories" sheetId="10" r:id="rId13"/>
+    <sheet name="Forest Type" sheetId="16" r:id="rId2"/>
+    <sheet name="Age Classes" sheetId="14" r:id="rId3"/>
+    <sheet name="Perennial Cropland Tyoe" sheetId="15" r:id="rId4"/>
+    <sheet name="Continent Type" sheetId="13" r:id="rId5"/>
+    <sheet name="Eco Zones" sheetId="12" r:id="rId6"/>
+    <sheet name="ClimateRegions" sheetId="3" r:id="rId7"/>
+    <sheet name="ClimateDomains" sheetId="4" r:id="rId8"/>
+    <sheet name="SoilTypes" sheetId="5" r:id="rId9"/>
+    <sheet name="SoilComposition" sheetId="6" r:id="rId10"/>
+    <sheet name="SoilStatus" sheetId="8" r:id="rId11"/>
+    <sheet name="NutrientType" sheetId="9" r:id="rId12"/>
+    <sheet name="LandCategories" sheetId="11" r:id="rId13"/>
+    <sheet name="LandSubcategories" sheetId="10" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="ipcc2006_unprotected.accdb" localSheetId="0" hidden="1">Countries!$A$1:$B$250</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="6" hidden="1">ClimateDomains!$A$1:$B$6</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="11" hidden="1">LandCategories!$A$1:$D$7</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="12" hidden="1">LandSubcategories!$A$1:$D$13</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="10" hidden="1">NutrientType!$A$1:$C$4</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="8" hidden="1">SoilComposition!$A$1:$B$4</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="9" hidden="1">SoilStatus!$A$1:$B$6</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="7" hidden="1">SoilTypes!$A$1:$D$12</definedName>
-    <definedName name="Query_from_IPCC2006_1" localSheetId="5" hidden="1">ClimateRegions!$A$1:$E$18</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="7" hidden="1">ClimateDomains!$A$1:$B$6</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="12" hidden="1">LandCategories!$A$1:$D$7</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="13" hidden="1">LandSubcategories!$A$1:$D$13</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="11" hidden="1">NutrientType!$A$1:$C$4</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="9" hidden="1">SoilComposition!$A$1:$B$4</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="10" hidden="1">SoilStatus!$A$1:$B$6</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="8" hidden="1">SoilTypes!$A$1:$D$12</definedName>
+    <definedName name="Query_from_IPCC2006_1" localSheetId="6" hidden="1">ClimateRegions!$A$1:$E$18</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -80,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="696">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="709">
   <si>
     <t>country_code</t>
   </si>
@@ -2168,6 +2180,45 @@
   </si>
   <si>
     <t>Multistorey system</t>
+  </si>
+  <si>
+    <t>spiece</t>
+  </si>
+  <si>
+    <t>leaf_type_id</t>
+  </si>
+  <si>
+    <t>ord</t>
+  </si>
+  <si>
+    <t>is_ws</t>
+  </si>
+  <si>
+    <t>Pinus</t>
+  </si>
+  <si>
+    <t>Larch</t>
+  </si>
+  <si>
+    <t>Firs and spruce</t>
+  </si>
+  <si>
+    <t>Other Coniferous</t>
+  </si>
+  <si>
+    <t>Eucalyptus</t>
+  </si>
+  <si>
+    <t>Tectona grandis</t>
+  </si>
+  <si>
+    <t>Other Broadleaf</t>
+  </si>
+  <si>
+    <t>Quercus</t>
+  </si>
+  <si>
+    <t>Mangroves</t>
   </si>
 </sst>
 </file>
@@ -5007,6 +5058,58 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>554</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -5074,7 +5177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -5137,7 +5240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -5257,7 +5360,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -5462,10 +5565,255 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C723BFD1-A5D9-41AD-95C0-23970B2B9436}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="41.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>697</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="str">
+        <f>CONCATENATE(B2,"(",'Forest Type'!A2,"','")</f>
+        <v>Pinus(1','</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="str">
+        <f>CONCATENATE(B3,"(",'Forest Type'!A3,"','")</f>
+        <v>Larch(2','</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="str">
+        <f>CONCATENATE(B4,"(",'Forest Type'!A4,"','")</f>
+        <v>Firs and spruce(3','</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="str">
+        <f>CONCATENATE(B5,"(",'Forest Type'!A5,"','")</f>
+        <v>Other Coniferous(4','</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="str">
+        <f>CONCATENATE(B6,"(",'Forest Type'!A6,"','")</f>
+        <v>Eucalyptus(5','</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="str">
+        <f>CONCATENATE(B7,"(",'Forest Type'!A7,"','")</f>
+        <v>Tectona grandis(6','</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="str">
+        <f>CONCATENATE(B8,"(",'Forest Type'!A8,"','")</f>
+        <v>Other Broadleaf(7','</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="str">
+        <f>CONCATENATE(B9,"(",'Forest Type'!A9,"','")</f>
+        <v>Quercus(8','</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="str">
+        <f>CONCATENATE(B10,"(",'Forest Type'!A10,"','")</f>
+        <v>User-defined(9','</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" t="str">
+        <f>CONCATENATE(B11,"(",'Forest Type'!A11,"','")</f>
+        <v>Mangroves(10','</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52778016-B9B5-4B52-9FDC-F11584770CB3}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -5568,12 +5916,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC711E2-8096-4A36-88C5-6F3DA6130B2B}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5716,7 +6064,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{919BDACE-FCC6-400C-9A65-B218A62077AD}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -5779,12 +6127,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850405B3-C0A5-40B7-89FC-3379D7DE377D}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D22"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5792,9 +6140,10 @@
     <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>500</v>
       </c>
@@ -5808,7 +6157,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -5821,8 +6170,12 @@
       <c r="D2" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>TAr(Tropical rain forest','2,wet: ≤ 3 months dry, during winter</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -5835,8 +6188,12 @@
       <c r="D3" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>TAwa(Tropical moist deciduous forest','4,mainly wet: 3-5 months dry, during winter</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -5849,8 +6206,12 @@
       <c r="D4" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>TAWb(Tropical dry forest','5,mainly dry: 5-8 months dry, during winter</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
@@ -5863,8 +6224,12 @@
       <c r="D5" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>TBSh(Tropical shrubland','6,semi-arid: evaporation &gt; precipitation</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
@@ -5877,8 +6242,12 @@
       <c r="D6" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>TBWh(Tropical desert','7,arid: all months dry</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8</v>
       </c>
@@ -5891,8 +6260,12 @@
       <c r="D7" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>TM(Tropical mountain systems','8,altitudes approximately &gt;1000 m, with local variations</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
@@ -5905,8 +6278,12 @@
       <c r="D8" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>SCf(Subtropical humid forest','9,humid: no dry season</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10</v>
       </c>
@@ -5919,8 +6296,12 @@
       <c r="D9" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>SCs(Subtropical dry forest','10,seasonally dry: winter rains, dry summer</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11</v>
       </c>
@@ -5933,8 +6314,12 @@
       <c r="D10" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>SBSh(Subtropical steppe','11,semi-arid: evaporation &gt;precipitation</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>12</v>
       </c>
@@ -5947,8 +6332,12 @@
       <c r="D11" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F11" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>SBWh(Subtropical desert','12,arid: all months dry</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>13</v>
       </c>
@@ -5961,8 +6350,12 @@
       <c r="D12" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F12" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>SM(Subtropical mountain systems','13,altitudes approximately 800 m- 1000 m</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>14</v>
       </c>
@@ -5975,8 +6368,12 @@
       <c r="D13" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F13" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>TeDo(Temperate oceanic forest','14,oceanic climate: coldest month &gt;0°C</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>17</v>
       </c>
@@ -5989,8 +6386,12 @@
       <c r="D14" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F14" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>TeDc(Temperate continental forest','17,continental climate: coldest month &lt;0°C</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>18</v>
       </c>
@@ -6003,8 +6404,12 @@
       <c r="D15" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F15" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>TeBSk(Temperate steppe','18,semi-arid: evaporation &gt; precipitation</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>19</v>
       </c>
@@ -6017,8 +6422,12 @@
       <c r="D16" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>TeBWk(Temperate desert','19,arid: all months dry</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20</v>
       </c>
@@ -6031,8 +6440,12 @@
       <c r="D17" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>TeM(Temperate mountain systems','20,altitudes approximately &gt;800 m</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>21</v>
       </c>
@@ -6045,8 +6458,12 @@
       <c r="D18" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>Ba(Boreal coniferous forest','21,coniferous dense forest dominant</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>22</v>
       </c>
@@ -6059,8 +6476,12 @@
       <c r="D19" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F19" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>Bb(Boreal tundra woodland','22,woodland and sparse forest dominant</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>23</v>
       </c>
@@ -6073,8 +6494,12 @@
       <c r="D20" t="s">
         <v>666</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>BM(Boreal mountain systems','23,altitudes approximately &gt;600 m</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>24</v>
       </c>
@@ -6087,8 +6512,12 @@
       <c r="D21" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F21" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>P(Polar','24,all months &lt;10°C</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>25</v>
       </c>
@@ -6100,6 +6529,10 @@
       </c>
       <c r="D22" t="s">
         <v>671</v>
+      </c>
+      <c r="F22" t="str">
+        <f>CONCATENATE( Table2[[#This Row],[code]],"(",Table2[[#This Row],[zone]],"','",Table2[[#This Row],[ID]],",",Table2[[#This Row],[zone_criteria]])</f>
+        <v>NA(User-defined','25,Not part of IPCC 2006 default classification</v>
       </c>
     </row>
   </sheetData>
@@ -6110,12 +6543,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E20"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6368,7 +6801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -6436,7 +6869,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -6607,56 +7040,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>500</v>
-      </c>
-      <c r="B1" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>554</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
IPCC export working first version
</commit_message>
<xml_diff>
--- a/collect-earth/collect-earth-app/src/main/java/org/openforis/collect/earth/ipcc/serialize/IPCC2006_nomenclatures.xlsx
+++ b/collect-earth/collect-earth-app/src/main/java/org/openforis/collect/earth/ipcc/serialize/IPCC2006_nomenclatures.xlsx
@@ -8,36 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfonso Sanchez-Paus\workspace\maven.1480939002496\collect-earth\collect-earth-app\src\main\java\org\openforis\collect\earth\ipcc\serialize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4650624-4E30-42AA-9DED-D35778FCC785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF68EFDC-64B3-4F43-AEDC-82CF08356018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries" sheetId="1" r:id="rId1"/>
     <sheet name="Forest Type" sheetId="16" r:id="rId2"/>
-    <sheet name="Age Classes" sheetId="14" r:id="rId3"/>
-    <sheet name="Perennial Cropland Tyoe" sheetId="15" r:id="rId4"/>
-    <sheet name="Continent Type" sheetId="13" r:id="rId5"/>
-    <sheet name="Eco Zones" sheetId="12" r:id="rId6"/>
-    <sheet name="ClimateRegions" sheetId="3" r:id="rId7"/>
-    <sheet name="ClimateDomains" sheetId="4" r:id="rId8"/>
-    <sheet name="SoilTypes" sheetId="5" r:id="rId9"/>
-    <sheet name="SoilComposition" sheetId="6" r:id="rId10"/>
-    <sheet name="SoilStatus" sheetId="8" r:id="rId11"/>
-    <sheet name="NutrientType" sheetId="9" r:id="rId12"/>
-    <sheet name="LandCategories" sheetId="11" r:id="rId13"/>
-    <sheet name="LandSubcategories" sheetId="10" r:id="rId14"/>
+    <sheet name="Growing stock level" sheetId="17" r:id="rId3"/>
+    <sheet name="Age Classes" sheetId="14" r:id="rId4"/>
+    <sheet name="Perennial Cropland Tyoe" sheetId="15" r:id="rId5"/>
+    <sheet name="Continent Type" sheetId="13" r:id="rId6"/>
+    <sheet name="Eco Zones" sheetId="12" r:id="rId7"/>
+    <sheet name="ClimateRegions" sheetId="3" r:id="rId8"/>
+    <sheet name="ClimateDomains" sheetId="4" r:id="rId9"/>
+    <sheet name="SoilTypes" sheetId="5" r:id="rId10"/>
+    <sheet name="SoilComposition" sheetId="6" r:id="rId11"/>
+    <sheet name="SoilStatus" sheetId="8" r:id="rId12"/>
+    <sheet name="NutrientType" sheetId="9" r:id="rId13"/>
+    <sheet name="LandCategories" sheetId="11" r:id="rId14"/>
+    <sheet name="LandSubcategories" sheetId="10" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="ipcc2006_unprotected.accdb" localSheetId="0" hidden="1">Countries!$A$1:$B$250</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="7" hidden="1">ClimateDomains!$A$1:$B$6</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="12" hidden="1">LandCategories!$A$1:$D$7</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="13" hidden="1">LandSubcategories!$A$1:$D$13</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="11" hidden="1">NutrientType!$A$1:$C$4</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="9" hidden="1">SoilComposition!$A$1:$B$4</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="10" hidden="1">SoilStatus!$A$1:$B$6</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="8" hidden="1">SoilTypes!$A$1:$D$12</definedName>
-    <definedName name="Query_from_IPCC2006_1" localSheetId="6" hidden="1">ClimateRegions!$A$1:$E$18</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="8" hidden="1">ClimateDomains!$A$1:$B$6</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="13" hidden="1">LandCategories!$A$1:$D$7</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="14" hidden="1">LandSubcategories!$A$1:$D$13</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="12" hidden="1">NutrientType!$A$1:$C$4</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="10" hidden="1">SoilComposition!$A$1:$B$4</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="11" hidden="1">SoilStatus!$A$1:$B$6</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="9" hidden="1">SoilTypes!$A$1:$D$12</definedName>
+    <definedName name="Query_from_IPCC2006_1" localSheetId="7" hidden="1">ClimateRegions!$A$1:$E$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -92,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="728">
   <si>
     <t>country_code</t>
   </si>
@@ -2219,13 +2220,70 @@
   </si>
   <si>
     <t>Mangroves</t>
+  </si>
+  <si>
+    <t>gsl_domain_id</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>&lt;20</t>
+  </si>
+  <si>
+    <t>21-50</t>
+  </si>
+  <si>
+    <t>51-100</t>
+  </si>
+  <si>
+    <t>&gt;100</t>
+  </si>
+  <si>
+    <t>21-40</t>
+  </si>
+  <si>
+    <t>41-100</t>
+  </si>
+  <si>
+    <t>101-200</t>
+  </si>
+  <si>
+    <t>&gt;200</t>
+  </si>
+  <si>
+    <t>41-80</t>
+  </si>
+  <si>
+    <t>&gt;80</t>
+  </si>
+  <si>
+    <t>&lt;10</t>
+  </si>
+  <si>
+    <t>10-20</t>
+  </si>
+  <si>
+    <t>41-60</t>
+  </si>
+  <si>
+    <t>61-80</t>
+  </si>
+  <si>
+    <t>81-120</t>
+  </si>
+  <si>
+    <t>121-200</t>
+  </si>
+  <si>
+    <t>gsl_domain_id is linked to the Climate Domain</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2242,6 +2300,11 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2312,8 +2375,8 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -2321,30 +2384,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2514,18 +2553,42 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="thin">
           <color indexed="8"/>
         </top>
         <bottom style="thin">
           <color indexed="22"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="8"/>
         </bottom>
       </border>
     </dxf>
@@ -2679,13 +2742,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{16E0E9C7-65DF-4425-9BFD-67C050E9A94B}" name="Table2" displayName="Table2" ref="A1:D22" totalsRowShown="0" dataDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{16E0E9C7-65DF-4425-9BFD-67C050E9A94B}" name="Table2" displayName="Table2" ref="A1:D22" totalsRowShown="0" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="A1:D22" xr:uid="{16E0E9C7-65DF-4425-9BFD-67C050E9A94B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{10BBFB9A-CB17-4714-AFB7-2CC595D5C8D5}" name="ID" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{683919AA-1BB9-47B2-8FFC-9CD6D4C65EE9}" name="zone" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{022147EC-8547-4886-BCC9-610D09966DE5}" name="code" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{7F111D13-1ADB-40B0-881A-328358F8C0E2}" name="zone_criteria" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{10BBFB9A-CB17-4714-AFB7-2CC595D5C8D5}" name="ID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{683919AA-1BB9-47B2-8FFC-9CD6D4C65EE9}" name="zone" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{022147EC-8547-4886-BCC9-610D09966DE5}" name="code" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{7F111D13-1ADB-40B0-881A-328358F8C0E2}" name="zone_criteria" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5058,6 +5121,179 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>536</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>537</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>538</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>539</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>540</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>541</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>542</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>543</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>544</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>546</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>548</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>550</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -5109,7 +5345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -5177,7 +5413,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -5240,7 +5476,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -5360,7 +5596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -5810,11 +6046,429 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C583C7-F8CC-489C-8442-F9F2E3C1DA8C}">
+  <dimension ref="A1:F36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>709</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F4" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>27</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>28</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>30</v>
+      </c>
+      <c r="B18" s="2">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>31</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>32</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>33</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>34</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>35</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>36</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>37</v>
+      </c>
+      <c r="B25" s="2">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>38</v>
+      </c>
+      <c r="B26" s="2">
+        <v>4</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>39</v>
+      </c>
+      <c r="B27" s="2">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>40</v>
+      </c>
+      <c r="B28" s="2">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>41</v>
+      </c>
+      <c r="B29" s="2">
+        <v>7</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>42</v>
+      </c>
+      <c r="B30" s="2">
+        <v>8</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>43</v>
+      </c>
+      <c r="B31" s="2">
+        <v>9</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>44</v>
+      </c>
+      <c r="B32" s="2">
+        <v>10</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>45</v>
+      </c>
+      <c r="B33" s="2">
+        <v>11</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>46</v>
+      </c>
+      <c r="B34" s="2">
+        <v>12</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>47</v>
+      </c>
+      <c r="B35" s="2">
+        <v>13</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>48</v>
+      </c>
+      <c r="B36" s="2">
+        <v>14</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52778016-B9B5-4B52-9FDC-F11584770CB3}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5916,11 +6570,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC711E2-8096-4A36-88C5-6F3DA6130B2B}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B13"/>
     </sheetView>
   </sheetViews>
@@ -6064,7 +6718,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{919BDACE-FCC6-400C-9A65-B218A62077AD}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -6127,7 +6781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850405B3-C0A5-40B7-89FC-3379D7DE377D}">
   <dimension ref="A1:F22"/>
   <sheetViews>
@@ -6543,7 +7197,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
@@ -6801,7 +7455,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -6867,177 +7521,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>500</v>
-      </c>
-      <c r="B1" t="s">
-        <v>534</v>
-      </c>
-      <c r="C1" t="s">
-        <v>535</v>
-      </c>
-      <c r="D1" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>536</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>537</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>538</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>539</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>540</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>541</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>542</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>543</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>544</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>546</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>548</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>550</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Generating data for IPCC
</commit_message>
<xml_diff>
--- a/collect-earth/collect-earth-app/src/main/java/org/openforis/collect/earth/ipcc/serialize/IPCC2006_nomenclatures.xlsx
+++ b/collect-earth/collect-earth-app/src/main/java/org/openforis/collect/earth/ipcc/serialize/IPCC2006_nomenclatures.xlsx
@@ -8,37 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfonso Sanchez-Paus\workspace\maven.1480939002496\collect-earth\collect-earth-app\src\main\java\org\openforis\collect\earth\ipcc\serialize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF68EFDC-64B3-4F43-AEDC-82CF08356018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C8E496-CE67-451A-A20E-AAA575E71D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="8" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries" sheetId="1" r:id="rId1"/>
     <sheet name="Forest Type" sheetId="16" r:id="rId2"/>
     <sheet name="Growing stock level" sheetId="17" r:id="rId3"/>
     <sheet name="Age Classes" sheetId="14" r:id="rId4"/>
-    <sheet name="Perennial Cropland Tyoe" sheetId="15" r:id="rId5"/>
-    <sheet name="Continent Type" sheetId="13" r:id="rId6"/>
-    <sheet name="Eco Zones" sheetId="12" r:id="rId7"/>
-    <sheet name="ClimateRegions" sheetId="3" r:id="rId8"/>
-    <sheet name="ClimateDomains" sheetId="4" r:id="rId9"/>
-    <sheet name="SoilTypes" sheetId="5" r:id="rId10"/>
-    <sheet name="SoilComposition" sheetId="6" r:id="rId11"/>
-    <sheet name="SoilStatus" sheetId="8" r:id="rId12"/>
-    <sheet name="NutrientType" sheetId="9" r:id="rId13"/>
-    <sheet name="LandCategories" sheetId="11" r:id="rId14"/>
-    <sheet name="LandSubcategories" sheetId="10" r:id="rId15"/>
+    <sheet name="Vegetation Tyoe Grassland" sheetId="18" r:id="rId5"/>
+    <sheet name="Perennial Cropland Tyoe" sheetId="15" r:id="rId6"/>
+    <sheet name="Continent Type" sheetId="13" r:id="rId7"/>
+    <sheet name="Eco Zones" sheetId="12" r:id="rId8"/>
+    <sheet name="ClimateRegions" sheetId="3" r:id="rId9"/>
+    <sheet name="ClimateDomains" sheetId="4" r:id="rId10"/>
+    <sheet name="SoilTypes" sheetId="5" r:id="rId11"/>
+    <sheet name="SoilComposition" sheetId="6" r:id="rId12"/>
+    <sheet name="SoilStatus" sheetId="8" r:id="rId13"/>
+    <sheet name="NutrientType" sheetId="9" r:id="rId14"/>
+    <sheet name="LandCategories" sheetId="11" r:id="rId15"/>
+    <sheet name="LandSubcategories" sheetId="10" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="ipcc2006_unprotected.accdb" localSheetId="0" hidden="1">Countries!$A$1:$B$250</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="8" hidden="1">ClimateDomains!$A$1:$B$6</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="13" hidden="1">LandCategories!$A$1:$D$7</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="14" hidden="1">LandSubcategories!$A$1:$D$13</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="12" hidden="1">NutrientType!$A$1:$C$4</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="10" hidden="1">SoilComposition!$A$1:$B$4</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="11" hidden="1">SoilStatus!$A$1:$B$6</definedName>
-    <definedName name="Query_from_IPCC2006" localSheetId="9" hidden="1">SoilTypes!$A$1:$D$12</definedName>
-    <definedName name="Query_from_IPCC2006_1" localSheetId="7" hidden="1">ClimateRegions!$A$1:$E$18</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="9" hidden="1">ClimateDomains!$A$1:$B$6</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="14" hidden="1">LandCategories!$A$1:$D$7</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="15" hidden="1">LandSubcategories!$A$1:$D$13</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="13" hidden="1">NutrientType!$A$1:$C$4</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="11" hidden="1">SoilComposition!$A$1:$B$4</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="12" hidden="1">SoilStatus!$A$1:$B$6</definedName>
+    <definedName name="Query_from_IPCC2006" localSheetId="10" hidden="1">SoilTypes!$A$1:$D$12</definedName>
+    <definedName name="Query_from_IPCC2006_1" localSheetId="8" hidden="1">ClimateRegions!$A$1:$E$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -93,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="752">
   <si>
     <t>country_code</t>
   </si>
@@ -2277,13 +2278,85 @@
   </si>
   <si>
     <t>gsl_domain_id is linked to the Climate Domain</t>
+  </si>
+  <si>
+    <t>vegetation_type</t>
+  </si>
+  <si>
+    <t>ratio_bgb_agb</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>Steppe</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>±150%</t>
+  </si>
+  <si>
+    <t>Tundra</t>
+  </si>
+  <si>
+    <t>TU</t>
+  </si>
+  <si>
+    <t>Prairie</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>Semi-Arid</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>±95%</t>
+  </si>
+  <si>
+    <t>Sub-Tropical</t>
+  </si>
+  <si>
+    <t>±130%</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>Woodland</t>
+  </si>
+  <si>
+    <t>±80%</t>
+  </si>
+  <si>
+    <t>Savannah</t>
+  </si>
+  <si>
+    <t>SV</t>
+  </si>
+  <si>
+    <t>Shrubland</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>±144%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2300,11 +2373,6 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -5121,6 +5189,74 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>533</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -5293,7 +5429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -5345,7 +5481,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -5413,7 +5549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -5476,7 +5612,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -5596,11 +5732,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6049,8 +6185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C583C7-F8CC-489C-8442-F9F2E3C1DA8C}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6468,7 +6604,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6571,6 +6707,221 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E2E4AA-557C-4B6A-8EEE-4082B2752ABB}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>728</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="E5" s="2">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="E6" s="2">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>19</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>19</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="E10" s="2">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>751</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC711E2-8096-4A36-88C5-6F3DA6130B2B}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -6718,12 +7069,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{919BDACE-FCC6-400C-9A65-B218A62077AD}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6781,7 +7132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850405B3-C0A5-40B7-89FC-3379D7DE377D}">
   <dimension ref="A1:F22"/>
   <sheetViews>
@@ -7197,7 +7548,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
@@ -7453,72 +7804,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>500</v>
-      </c>
-      <c r="B1" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>533</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>